<commit_message>
Update of Excel Matrix
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/Project_1_ood/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{662D510B-8986-41B1-A741-49515041D2FB}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1156CC8-3997-476B-968F-0BD7793B7FC8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>Data Set</t>
-  </si>
-  <si>
     <t>IMDB</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>E (FL+1)</t>
   </si>
   <si>
-    <t>DM (FL)</t>
-  </si>
-  <si>
     <t>TRUSTED (FPM)</t>
   </si>
   <si>
@@ -90,6 +84,15 @@
   </si>
   <si>
     <t>AUROC, AUPR-IN, AUPR-OUT, FPR, ERR</t>
+  </si>
+  <si>
+    <t>DIRW (FL)</t>
+  </si>
+  <si>
+    <t>OOD set</t>
+  </si>
+  <si>
+    <t>Training/test set</t>
   </si>
 </sst>
 </file>
@@ -142,32 +145,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -191,19 +174,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -222,6 +192,45 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -231,48 +240,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,10 +293,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,151 +592,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87897C9-3237-4ECE-9BA5-6ACBCCECEBEF}">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E1" s="15" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E1:H1"/>
+  <mergeCells count="1">
+    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update of Matrix and tasks
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1156CC8-3997-476B-968F-0BD7793B7FC8}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81586795-8CEB-4997-8E6E-9AE01215FF82}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -50,49 +50,76 @@
     <t>SST2</t>
   </si>
   <si>
-    <t>Pretrained encoders</t>
-  </si>
-  <si>
     <t>BERT</t>
   </si>
   <si>
-    <t>Dist</t>
-  </si>
-  <si>
-    <t>RoB</t>
-  </si>
-  <si>
-    <t>OOD detectors</t>
-  </si>
-  <si>
-    <t>MSP (Soft)</t>
-  </si>
-  <si>
-    <t>E (FL+1)</t>
-  </si>
-  <si>
-    <t>TRUSTED (FPM)</t>
-  </si>
-  <si>
-    <t>Implemented</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance metrics: </t>
-  </si>
-  <si>
-    <t>AUROC, AUPR-IN, AUPR-OUT, FPR, ERR</t>
-  </si>
-  <si>
-    <t>DIRW (FL)</t>
-  </si>
-  <si>
-    <t>OOD set</t>
-  </si>
-  <si>
-    <t>Training/test set</t>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
+  <si>
+    <t>Softmax</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>FL+1</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>FPM</t>
+  </si>
+  <si>
+    <t>DIRW</t>
+  </si>
+  <si>
+    <t>TRUSTED</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>AUROC</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>ERR</t>
+  </si>
+  <si>
+    <t>AUPR</t>
+  </si>
+  <si>
+    <t>1. Adapter BERT pour produire les méthodes d'agrégation.</t>
+  </si>
+  <si>
+    <t>2. Implémenter les scores.</t>
+  </si>
+  <si>
+    <t>3. Implémenter les mesures de performance.</t>
+  </si>
+  <si>
+    <t>4. Remplir la matrice des résultats.</t>
   </si>
 </sst>
 </file>
@@ -116,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,14 +156,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -145,54 +166,122 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -201,37 +290,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -240,44 +305,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,6 +348,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,123 +651,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87897C9-3237-4ECE-9BA5-6ACBCCECEBEF}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
-        <v>18</v>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
-        <v>17</v>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="8" t="s">
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
+      <c r="D14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C5:F5"/>
+  <mergeCells count="3">
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B7:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel and next steps
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81586795-8CEB-4997-8E6E-9AE01215FF82}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73FE2869-3FC4-4EC5-825D-1018986CBD5D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>4. Remplir la matrice des résultats.</t>
+  </si>
+  <si>
+    <t>5. Rédiger le document overleaf</t>
   </si>
 </sst>
 </file>
@@ -309,9 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,18 +321,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87897C9-3237-4ECE-9BA5-6ACBCCECEBEF}">
-  <dimension ref="B1:H20"/>
+  <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,30 +694,30 @@
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -726,10 +729,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
@@ -739,11 +742,11 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -752,33 +755,33 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="8"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="8"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="8"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -787,31 +790,31 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="8"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="8"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
@@ -831,6 +834,11 @@
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel and BERT features functions
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73FE2869-3FC4-4EC5-825D-1018986CBD5D}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE57283-822C-4F91-BC74-FA1AD24E093D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>TRUSTED</t>
-  </si>
-  <si>
-    <t>PM</t>
   </si>
   <si>
     <t>AUROC</t>
@@ -656,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87897C9-3237-4ECE-9BA5-6ACBCCECEBEF}">
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +675,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -686,7 +683,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -704,16 +701,16 @@
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -809,7 +806,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -818,27 +815,27 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add OOD detection with MSP and Energy score
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{99B0218C-18B0-4483-A6E6-54E425E861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE57283-822C-4F91-BC74-FA1AD24E093D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2805F6B5-4A4B-4F7E-B6F6-9822CC64C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -80,13 +80,13 @@
     <t>FL</t>
   </si>
   <si>
-    <t>FPM</t>
-  </si>
-  <si>
     <t>DIRW</t>
   </si>
   <si>
     <t>TRUSTED</t>
+  </si>
+  <si>
+    <t>PM</t>
   </si>
   <si>
     <t>AUROC</t>
@@ -350,12 +350,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -651,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87897C9-3237-4ECE-9BA5-6ACBCCECEBEF}">
-  <dimension ref="B1:H21"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,10 +745,18 @@
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="6"/>
+      <c r="E9" s="2">
+        <v>87.4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G9" s="2">
+        <v>15.1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
@@ -760,16 +764,26 @@
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="2">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F10" s="2">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="H10" s="6">
+        <v>20.9</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -778,71 +792,58 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
-      <c r="C12" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="7" t="s">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="12"/>
+      <c r="C13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B7:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Energy and softmax results
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d91261b4064fd49f/Documentos/NLP/OOD_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2805F6B5-4A4B-4F7E-B6F6-9822CC64C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{2805F6B5-4A4B-4F7E-B6F6-9822CC64C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415C1808-6997-414E-A532-C7C66A2CF914}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{323ADEE6-9D40-4FB4-91BB-9B54E302B6D0}"/>
   </bookViews>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,7 +650,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,10 +719,18 @@
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="6"/>
+      <c r="E7" s="2">
+        <v>76.7</v>
+      </c>
+      <c r="F7" s="2">
+        <v>49.8</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="H7" s="6">
+        <v>27.3</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
@@ -732,10 +740,18 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="6"/>
+      <c r="E8" s="2">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="F8" s="2">
+        <v>54.8</v>
+      </c>
+      <c r="G8" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>26.4</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>

</xml_diff>